<commit_message>
기존 [Pass_List] 시트를 [Pass_List / Pass_Level] 로 분할
</commit_message>
<xml_diff>
--- a/Client/Assets/11. GameData/Pass.xlsx
+++ b/Client/Assets/11. GameData/Pass.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcmbb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fda0e400ac064334/Be_greatman/01 Project/★미야옹 파이터즈 클럽/09 Season Pass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5CC2E3-F962-41D9-A688-767054B3CBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{3B5CC2E3-F962-41D9-A688-767054B3CBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83034FA2-1FAA-475E-AFEB-35CC59CADDBB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="535" activeTab="2" xr2:uid="{E3B10073-6739-413D-9047-29D24A9ED330}"/>
   </bookViews>
   <sheets>
     <sheet name="Pass_Info" sheetId="4" r:id="rId1"/>
-    <sheet name="Pass_List" sheetId="1" r:id="rId2"/>
-    <sheet name="Pass_Mission" sheetId="2" r:id="rId3"/>
+    <sheet name="Pass_List" sheetId="5" r:id="rId2"/>
+    <sheet name="Pass_Level" sheetId="1" r:id="rId3"/>
+    <sheet name="Pass_Mission" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -148,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -178,9 +179,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[시즌1] 미야옹 패스</t>
-  </si>
-  <si>
     <t>Reward_Item_Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -461,6 +459,10 @@
   </si>
   <si>
     <t>Required_Item_Grade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -468,7 +470,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,12 +502,6 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -589,7 +585,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -611,17 +607,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1029,7 +1019,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1042,123 +1032,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="12" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="2" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="8" t="s">
+    <row r="7" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="8" t="s">
+    <row r="9" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="10" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1170,31 +1160,78 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC616978-B69C-4F7D-8301-6F88E773EBCB}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="3">
+        <v>601</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4">
+        <v>45573</v>
+      </c>
+      <c r="D2" s="4">
+        <v>72686</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A74E4F3-3BB8-4CF3-AC0A-3F86C309575D}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.69921875" customWidth="1"/>
-    <col min="2" max="2" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" customWidth="1"/>
     <col min="4" max="4" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.69921875" customWidth="1"/>
+    <col min="5" max="5" width="10.09765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.69921875" customWidth="1"/>
+    <col min="8" max="8" width="12.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1203,27 +1240,21 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>60101</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
+      <c r="B2" s="3">
+        <v>601</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -1234,25 +1265,19 @@
       <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>100001</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>800</v>
       </c>
-      <c r="H2" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I2" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>60102</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
+      <c r="B3" s="3">
+        <v>601</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -1263,25 +1288,19 @@
       <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>100001</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>800</v>
       </c>
-      <c r="H3" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I3" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>60103</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
+      <c r="B4" s="3">
+        <v>601</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -1295,22 +1314,16 @@
       <c r="F4">
         <v>341003</v>
       </c>
-      <c r="G4" s="9">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I4" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>60104</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
+      <c r="B5" s="3">
+        <v>601</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
@@ -1321,25 +1334,19 @@
       <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>100001</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>800</v>
       </c>
-      <c r="H5" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I5" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>60105</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
+      <c r="B6" s="3">
+        <v>601</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -1350,25 +1357,19 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>100001</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>800</v>
       </c>
-      <c r="H6" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I6" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>60106</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
+      <c r="B7" s="3">
+        <v>601</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
@@ -1382,22 +1383,16 @@
       <c r="F7">
         <v>341017</v>
       </c>
-      <c r="G7" s="9">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I7" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>60107</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
+      <c r="B8" s="3">
+        <v>601</v>
       </c>
       <c r="C8" s="3">
         <v>7</v>
@@ -1408,25 +1403,19 @@
       <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>100001</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>800</v>
       </c>
-      <c r="H8" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I8" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>60108</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
+      <c r="B9" s="3">
+        <v>601</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
@@ -1437,25 +1426,19 @@
       <c r="E9" s="3">
         <v>1</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="11">
         <v>341019</v>
       </c>
-      <c r="G9" s="9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I9" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>60109</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
+      <c r="B10" s="3">
+        <v>601</v>
       </c>
       <c r="C10" s="3">
         <v>9</v>
@@ -1469,22 +1452,16 @@
       <c r="F10">
         <v>341006</v>
       </c>
-      <c r="G10" s="9">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I10" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>60110</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
+      <c r="B11" s="3">
+        <v>601</v>
       </c>
       <c r="C11" s="3">
         <v>10</v>
@@ -1495,262 +1472,208 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>201019</v>
       </c>
-      <c r="G11" s="9">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
-        <v>45573</v>
-      </c>
-      <c r="I11" s="4">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>60111</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>2</v>
+      <c r="B12" s="3">
+        <v>601</v>
       </c>
       <c r="C12" s="3">
         <v>11</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>100</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>100001</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>800</v>
       </c>
-      <c r="H12" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I12" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>60112</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>2</v>
+      <c r="B13" s="3">
+        <v>601</v>
       </c>
       <c r="C13" s="3">
         <v>12</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>100</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>100001</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>800</v>
       </c>
-      <c r="H13" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I13" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>60113</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>7</v>
+      <c r="B14" s="3">
+        <v>601</v>
       </c>
       <c r="C14" s="3">
         <v>13</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>100</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>341023</v>
       </c>
-      <c r="G14" s="9">
-        <v>1</v>
-      </c>
-      <c r="H14" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I14" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>60114</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>7</v>
+      <c r="B15" s="3">
+        <v>601</v>
       </c>
       <c r="C15" s="3">
         <v>14</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>100</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>100001</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>800</v>
       </c>
-      <c r="H15" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I15" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>60115</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
+      <c r="B16" s="3">
+        <v>601</v>
       </c>
       <c r="C16" s="3">
         <v>15</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>100</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>100001</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <v>800</v>
       </c>
-      <c r="H16" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I16" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>60116</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>7</v>
+      <c r="B17" s="3">
+        <v>601</v>
       </c>
       <c r="C17" s="3">
         <v>16</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>100</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>341027</v>
       </c>
-      <c r="G17" s="9">
-        <v>1</v>
-      </c>
-      <c r="H17" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I17" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>60117</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>7</v>
+      <c r="B18" s="3">
+        <v>601</v>
       </c>
       <c r="C18" s="3">
         <v>17</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>100</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>100001</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <v>800</v>
       </c>
-      <c r="H18" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I18" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>60118</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>7</v>
+      <c r="B19" s="3">
+        <v>601</v>
       </c>
       <c r="C19" s="3">
         <v>18</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <v>100</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>100001</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>800</v>
       </c>
-      <c r="H19" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I19" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>60119</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>7</v>
+      <c r="B20" s="3">
+        <v>601</v>
       </c>
       <c r="C20" s="3">
         <v>19</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>100</v>
       </c>
       <c r="E20" s="3">
@@ -1759,80 +1682,62 @@
       <c r="F20">
         <v>313001</v>
       </c>
-      <c r="G20" s="9">
-        <v>1</v>
-      </c>
-      <c r="H20" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I20" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>60120</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>7</v>
+      <c r="B21" s="3">
+        <v>601</v>
       </c>
       <c r="C21" s="3">
         <v>20</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <v>100</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>100002</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>1500</v>
       </c>
-      <c r="H21" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I21" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>60121</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>7</v>
+      <c r="B22" s="3">
+        <v>601</v>
       </c>
       <c r="C22" s="3">
         <v>21</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="7">
         <v>100</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="8">
         <v>100001</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="8">
         <v>500</v>
       </c>
-      <c r="H22" s="10">
-        <v>45573</v>
-      </c>
-      <c r="I22" s="10">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="5">
         <v>60201</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>2</v>
+      <c r="B23" s="5">
+        <v>601</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
@@ -1849,19 +1754,13 @@
       <c r="G23" s="6">
         <v>50</v>
       </c>
-      <c r="H23" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I23" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="5">
         <v>60202</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>2</v>
+      <c r="B24" s="5">
+        <v>601</v>
       </c>
       <c r="C24" s="5">
         <v>2</v>
@@ -1878,19 +1777,13 @@
       <c r="G24" s="6">
         <v>50</v>
       </c>
-      <c r="H24" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I24" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="5">
         <v>60203</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>7</v>
+      <c r="B25" s="5">
+        <v>601</v>
       </c>
       <c r="C25" s="5">
         <v>3</v>
@@ -1907,19 +1800,13 @@
       <c r="G25" s="6">
         <v>1</v>
       </c>
-      <c r="H25" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I25" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="5">
         <v>60204</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>7</v>
+      <c r="B26" s="5">
+        <v>601</v>
       </c>
       <c r="C26" s="5">
         <v>4</v>
@@ -1936,19 +1823,13 @@
       <c r="G26" s="6">
         <v>50</v>
       </c>
-      <c r="H26" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I26" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="5">
         <v>60205</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>7</v>
+      <c r="B27" s="5">
+        <v>601</v>
       </c>
       <c r="C27" s="5">
         <v>5</v>
@@ -1965,19 +1846,13 @@
       <c r="G27" s="6">
         <v>50</v>
       </c>
-      <c r="H27" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I27" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="5">
         <v>60206</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>7</v>
+      <c r="B28" s="5">
+        <v>601</v>
       </c>
       <c r="C28" s="5">
         <v>6</v>
@@ -1994,19 +1869,13 @@
       <c r="G28" s="6">
         <v>1</v>
       </c>
-      <c r="H28" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I28" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="5">
         <v>60207</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>7</v>
+      <c r="B29" s="5">
+        <v>601</v>
       </c>
       <c r="C29" s="5">
         <v>7</v>
@@ -2023,19 +1892,13 @@
       <c r="G29" s="6">
         <v>50</v>
       </c>
-      <c r="H29" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I29" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="5">
         <v>60208</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>7</v>
+      <c r="B30" s="5">
+        <v>601</v>
       </c>
       <c r="C30" s="5">
         <v>8</v>
@@ -2052,19 +1915,13 @@
       <c r="G30" s="6">
         <v>50</v>
       </c>
-      <c r="H30" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I30" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="5">
         <v>60209</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>7</v>
+      <c r="B31" s="5">
+        <v>601</v>
       </c>
       <c r="C31" s="5">
         <v>9</v>
@@ -2081,19 +1938,13 @@
       <c r="G31" s="6">
         <v>1</v>
       </c>
-      <c r="H31" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I31" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="5">
         <v>60210</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>7</v>
+      <c r="B32" s="5">
+        <v>601</v>
       </c>
       <c r="C32" s="5">
         <v>10</v>
@@ -2110,19 +1961,13 @@
       <c r="G32" s="6">
         <v>1</v>
       </c>
-      <c r="H32" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I32" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="5">
         <v>60211</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>2</v>
+      <c r="B33" s="5">
+        <v>601</v>
       </c>
       <c r="C33" s="5">
         <v>11</v>
@@ -2139,19 +1984,13 @@
       <c r="G33" s="6">
         <v>50</v>
       </c>
-      <c r="H33" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I33" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" s="5">
         <v>60212</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>2</v>
+      <c r="B34" s="5">
+        <v>601</v>
       </c>
       <c r="C34" s="5">
         <v>12</v>
@@ -2168,19 +2007,13 @@
       <c r="G34" s="6">
         <v>50</v>
       </c>
-      <c r="H34" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I34" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="5">
         <v>60213</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>7</v>
+      <c r="B35" s="5">
+        <v>601</v>
       </c>
       <c r="C35" s="5">
         <v>13</v>
@@ -2197,19 +2030,13 @@
       <c r="G35" s="6">
         <v>1</v>
       </c>
-      <c r="H35" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I35" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="5">
         <v>60214</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>7</v>
+      <c r="B36" s="5">
+        <v>601</v>
       </c>
       <c r="C36" s="5">
         <v>14</v>
@@ -2226,19 +2053,13 @@
       <c r="G36" s="6">
         <v>50</v>
       </c>
-      <c r="H36" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I36" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="5">
         <v>60215</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>7</v>
+      <c r="B37" s="5">
+        <v>601</v>
       </c>
       <c r="C37" s="5">
         <v>15</v>
@@ -2255,19 +2076,13 @@
       <c r="G37" s="6">
         <v>50</v>
       </c>
-      <c r="H37" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I37" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" s="5">
         <v>60216</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>7</v>
+      <c r="B38" s="5">
+        <v>601</v>
       </c>
       <c r="C38" s="5">
         <v>16</v>
@@ -2284,19 +2099,13 @@
       <c r="G38" s="6">
         <v>1</v>
       </c>
-      <c r="H38" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I38" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="5">
         <v>60217</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>7</v>
+      <c r="B39" s="5">
+        <v>601</v>
       </c>
       <c r="C39" s="5">
         <v>17</v>
@@ -2313,19 +2122,13 @@
       <c r="G39" s="6">
         <v>50</v>
       </c>
-      <c r="H39" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I39" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="5">
         <v>60218</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>7</v>
+      <c r="B40" s="5">
+        <v>601</v>
       </c>
       <c r="C40" s="5">
         <v>18</v>
@@ -2342,19 +2145,13 @@
       <c r="G40" s="6">
         <v>50</v>
       </c>
-      <c r="H40" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I40" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="5">
         <v>60219</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>7</v>
+      <c r="B41" s="5">
+        <v>601</v>
       </c>
       <c r="C41" s="5">
         <v>19</v>
@@ -2371,19 +2168,13 @@
       <c r="G41" s="6">
         <v>1</v>
       </c>
-      <c r="H41" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I41" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="5">
         <v>60220</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>7</v>
+      <c r="B42" s="5">
+        <v>601</v>
       </c>
       <c r="C42" s="5">
         <v>20</v>
@@ -2400,19 +2191,13 @@
       <c r="G42" s="6">
         <v>1</v>
       </c>
-      <c r="H42" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I42" s="7">
-        <v>72686</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="5">
         <v>60221</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>7</v>
+      <c r="B43" s="5">
+        <v>601</v>
       </c>
       <c r="C43" s="5">
         <v>21</v>
@@ -2428,12 +2213,6 @@
       </c>
       <c r="G43" s="6">
         <v>30</v>
-      </c>
-      <c r="H43" s="7">
-        <v>45573</v>
-      </c>
-      <c r="I43" s="7">
-        <v>72686</v>
       </c>
     </row>
   </sheetData>
@@ -2443,11 +2222,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4561621-BAF4-4FB5-8F15-B71B1A49C200}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
@@ -2482,302 +2261,302 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2" s="7">
+        <v>51011</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7">
+        <v>15</v>
+      </c>
+      <c r="K2" s="7">
+        <v>100001</v>
+      </c>
+      <c r="L2" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" s="7">
+        <v>51021</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7">
+        <v>3</v>
+      </c>
+      <c r="J3" s="7">
+        <v>15</v>
+      </c>
+      <c r="K3" s="7">
+        <v>100001</v>
+      </c>
+      <c r="L3" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" s="7">
+        <v>51031</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7">
+        <v>15</v>
+      </c>
+      <c r="K4" s="7">
+        <v>100001</v>
+      </c>
+      <c r="L4" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" s="7">
+        <v>51041</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="G5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>20</v>
+      </c>
+      <c r="K5" s="7">
+        <v>100001</v>
+      </c>
+      <c r="L5" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A6" s="7">
+        <v>51051</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7">
+        <v>3</v>
+      </c>
+      <c r="J6" s="7">
+        <v>20</v>
+      </c>
+      <c r="K6" s="7">
+        <v>100001</v>
+      </c>
+      <c r="L6" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" s="7">
+        <v>51061</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="7">
+        <v>20</v>
+      </c>
+      <c r="K7" s="7">
+        <v>100001</v>
+      </c>
+      <c r="L7" s="7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" s="7">
+        <v>51071</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7">
+        <v>7</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" s="8">
-        <v>51011</v>
-      </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="8">
-        <v>0</v>
-      </c>
-      <c r="I2" s="8">
-        <v>1</v>
-      </c>
-      <c r="J2" s="8">
-        <v>15</v>
-      </c>
-      <c r="K2" s="8">
+      <c r="J8" s="7">
+        <v>20</v>
+      </c>
+      <c r="K8" s="7">
         <v>100001</v>
       </c>
-      <c r="L2" s="8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="8">
-        <v>51021</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>3</v>
-      </c>
-      <c r="J3" s="8">
-        <v>15</v>
-      </c>
-      <c r="K3" s="8">
-        <v>100001</v>
-      </c>
-      <c r="L3" s="8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="8">
-        <v>51031</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0</v>
-      </c>
-      <c r="I4" s="8">
-        <v>3</v>
-      </c>
-      <c r="J4" s="8">
-        <v>15</v>
-      </c>
-      <c r="K4" s="8">
-        <v>100001</v>
-      </c>
-      <c r="L4" s="8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="8">
-        <v>51041</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
-        <v>4</v>
-      </c>
-      <c r="D5" s="8">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1</v>
-      </c>
-      <c r="J5" s="8">
-        <v>20</v>
-      </c>
-      <c r="K5" s="8">
-        <v>100001</v>
-      </c>
-      <c r="L5" s="8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="8">
-        <v>51051</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8">
-        <v>5</v>
-      </c>
-      <c r="D6" s="8">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8">
-        <v>3</v>
-      </c>
-      <c r="J6" s="8">
-        <v>20</v>
-      </c>
-      <c r="K6" s="8">
-        <v>100001</v>
-      </c>
-      <c r="L6" s="8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="8">
-        <v>51061</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8">
-        <v>6</v>
-      </c>
-      <c r="D7" s="8">
-        <v>6</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>5</v>
-      </c>
-      <c r="J7" s="8">
-        <v>20</v>
-      </c>
-      <c r="K7" s="8">
-        <v>100001</v>
-      </c>
-      <c r="L7" s="8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="8">
-        <v>51071</v>
-      </c>
-      <c r="B8" s="8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="8">
-        <v>7</v>
-      </c>
-      <c r="D8" s="8">
-        <v>7</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="8">
-        <v>10</v>
-      </c>
-      <c r="J8" s="8">
-        <v>20</v>
-      </c>
-      <c r="K8" s="8">
-        <v>100001</v>
-      </c>
-      <c r="L8" s="8">
+      <c r="L8" s="7">
         <v>500</v>
       </c>
     </row>
@@ -2798,10 +2577,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="5">
         <v>0</v>
@@ -2836,10 +2615,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="5">
         <v>0</v>
@@ -2874,10 +2653,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="5">
         <v>0</v>
@@ -2912,10 +2691,10 @@
         <v>4</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="H12" s="5">
         <v>0</v>
@@ -2950,10 +2729,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="5">
         <v>0</v>
@@ -2988,10 +2767,10 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" s="5">
         <v>0</v>
@@ -3026,10 +2805,10 @@
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="5">
         <v>0</v>
@@ -3064,10 +2843,10 @@
         <v>4</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="5">
         <v>0</v>
@@ -3102,10 +2881,10 @@
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H17" s="5">
         <v>0</v>
@@ -3140,10 +2919,10 @@
         <v>2</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18" s="5">
         <v>0</v>
@@ -3178,10 +2957,10 @@
         <v>3</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H19" s="5">
         <v>0</v>
@@ -3216,10 +2995,10 @@
         <v>1</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H20" s="5">
         <v>0</v>
@@ -3254,10 +3033,10 @@
         <v>2</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21" s="5">
         <v>0</v>
@@ -3292,10 +3071,10 @@
         <v>3</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H22" s="5">
         <v>0</v>
@@ -3330,10 +3109,10 @@
         <v>4</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H23" s="5">
         <v>0</v>
@@ -3368,10 +3147,10 @@
         <v>5</v>
       </c>
       <c r="F24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="H24" s="5">
         <v>0</v>
@@ -3406,10 +3185,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="H25" s="5">
         <v>0</v>
@@ -3444,10 +3223,10 @@
         <v>2</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H26" s="5">
         <v>0</v>
@@ -3482,10 +3261,10 @@
         <v>3</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H27" s="5">
         <v>0</v>
@@ -3520,10 +3299,10 @@
         <v>1</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H28" s="5">
         <v>0</v>
@@ -3558,10 +3337,10 @@
         <v>2</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H29" s="5">
         <v>0</v>
@@ -3596,10 +3375,10 @@
         <v>3</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H30" s="5">
         <v>0</v>
@@ -3634,10 +3413,10 @@
         <v>4</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H31" s="5">
         <v>0</v>
@@ -3672,10 +3451,10 @@
         <v>5</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="H32" s="5">
         <v>0</v>
@@ -3710,10 +3489,10 @@
         <v>1</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H33" s="5">
         <v>0</v>
@@ -3748,10 +3527,10 @@
         <v>2</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="H34" s="5">
         <v>0</v>
@@ -3786,10 +3565,10 @@
         <v>3</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H35" s="5">
         <v>0</v>
@@ -3824,10 +3603,10 @@
         <v>1</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H36" s="5">
         <v>3</v>
@@ -3862,10 +3641,10 @@
         <v>1</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H37" s="5">
         <v>2</v>

</xml_diff>